<commit_message>
Updated cell size analyses
</commit_message>
<xml_diff>
--- a/data/SEM_Stein_data/SEM_Stein_cell.diams.TOOLS.xlsx
+++ b/data/SEM_Stein_data/SEM_Stein_cell.diams.TOOLS.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmoge\GitHub\MinimalCell\data\SEM_Stein_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE48C43-1576-4B98-B544-F751CF5A84EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5C577E-5B66-49ED-8463-3E3B3E6AD574}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="3780" windowWidth="16005" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20715" yWindow="4710" windowWidth="16005" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9" sheetId="12" r:id="rId1"/>
-    <sheet name="1" sheetId="11" r:id="rId2"/>
-    <sheet name="13" sheetId="10" r:id="rId3"/>
-    <sheet name="6" sheetId="9" r:id="rId4"/>
-    <sheet name="3" sheetId="8" r:id="rId5"/>
-    <sheet name="10" sheetId="7" r:id="rId6"/>
-    <sheet name="17" sheetId="5" r:id="rId7"/>
-    <sheet name="16" sheetId="3" r:id="rId8"/>
-    <sheet name="4" sheetId="2" r:id="rId9"/>
-    <sheet name="19" sheetId="1" r:id="rId10"/>
-    <sheet name="11" sheetId="4" r:id="rId11"/>
-    <sheet name="8" sheetId="6" r:id="rId12"/>
+    <sheet name="summarized" sheetId="13" r:id="rId2"/>
+    <sheet name="1" sheetId="11" r:id="rId3"/>
+    <sheet name="13" sheetId="10" r:id="rId4"/>
+    <sheet name="6" sheetId="9" r:id="rId5"/>
+    <sheet name="3" sheetId="8" r:id="rId6"/>
+    <sheet name="10" sheetId="7" r:id="rId7"/>
+    <sheet name="17" sheetId="5" r:id="rId8"/>
+    <sheet name="16" sheetId="3" r:id="rId9"/>
+    <sheet name="4" sheetId="2" r:id="rId10"/>
+    <sheet name="19" sheetId="1" r:id="rId11"/>
+    <sheet name="11" sheetId="4" r:id="rId12"/>
+    <sheet name="8" sheetId="6" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -392,7 +393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EEE6844-91BF-4DB6-A088-320516B397B3}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:G45"/>
     </sheetView>
   </sheetViews>
@@ -1525,6 +1526,1792 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C4EBE4-8D22-4729-ACC1-DF5E7929C6E8}">
+  <dimension ref="A1:G77"/>
+  <sheetViews>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G77"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C2">
+        <v>26818.952000000001</v>
+      </c>
+      <c r="D2">
+        <v>16136</v>
+      </c>
+      <c r="E2">
+        <v>45741</v>
+      </c>
+      <c r="F2">
+        <v>-90</v>
+      </c>
+      <c r="G2">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C3">
+        <v>31030.241999999998</v>
+      </c>
+      <c r="D3">
+        <v>13256.61</v>
+      </c>
+      <c r="E3">
+        <v>65504</v>
+      </c>
+      <c r="F3">
+        <v>-91.456000000000003</v>
+      </c>
+      <c r="G3">
+        <v>0.61499999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C4">
+        <v>38263.019</v>
+      </c>
+      <c r="D4">
+        <v>20619.553</v>
+      </c>
+      <c r="E4">
+        <v>65530</v>
+      </c>
+      <c r="F4">
+        <v>-90.754000000000005</v>
+      </c>
+      <c r="G4">
+        <v>0.79200000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C5">
+        <v>26915.843000000001</v>
+      </c>
+      <c r="D5">
+        <v>9787</v>
+      </c>
+      <c r="E5">
+        <v>65068</v>
+      </c>
+      <c r="F5">
+        <v>-89.575999999999993</v>
+      </c>
+      <c r="G5">
+        <v>0.70299999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C6">
+        <v>35671.421000000002</v>
+      </c>
+      <c r="D6">
+        <v>17189</v>
+      </c>
+      <c r="E6">
+        <v>65012.940999999999</v>
+      </c>
+      <c r="F6">
+        <v>-89.144999999999996</v>
+      </c>
+      <c r="G6">
+        <v>0.69799999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C7">
+        <v>30179.966</v>
+      </c>
+      <c r="D7">
+        <v>17040.403999999999</v>
+      </c>
+      <c r="E7">
+        <v>56415.858999999997</v>
+      </c>
+      <c r="F7">
+        <v>-79.478999999999999</v>
+      </c>
+      <c r="G7">
+        <v>0.74199999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C8">
+        <v>18614.136999999999</v>
+      </c>
+      <c r="D8">
+        <v>11648.511</v>
+      </c>
+      <c r="E8">
+        <v>27521</v>
+      </c>
+      <c r="F8">
+        <v>-91.218999999999994</v>
+      </c>
+      <c r="G8">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C9">
+        <v>18364.919999999998</v>
+      </c>
+      <c r="D9">
+        <v>12653.067999999999</v>
+      </c>
+      <c r="E9">
+        <v>28810.9</v>
+      </c>
+      <c r="F9">
+        <v>-89.125</v>
+      </c>
+      <c r="G9">
+        <v>0.68200000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C10">
+        <v>25063.035</v>
+      </c>
+      <c r="D10">
+        <v>12794</v>
+      </c>
+      <c r="E10">
+        <v>50928.983999999997</v>
+      </c>
+      <c r="F10">
+        <v>-88.543999999999997</v>
+      </c>
+      <c r="G10">
+        <v>0.61499999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>29180.918000000001</v>
+      </c>
+      <c r="D11">
+        <v>13566.919</v>
+      </c>
+      <c r="E11">
+        <v>55846.195</v>
+      </c>
+      <c r="F11">
+        <v>-88.137</v>
+      </c>
+      <c r="G11">
+        <v>0.64100000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C12">
+        <v>26569.732</v>
+      </c>
+      <c r="D12">
+        <v>5985</v>
+      </c>
+      <c r="E12">
+        <v>49784.866999999998</v>
+      </c>
+      <c r="F12">
+        <v>-90.444000000000003</v>
+      </c>
+      <c r="G12">
+        <v>0.67200000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C13">
+        <v>26378.094000000001</v>
+      </c>
+      <c r="D13">
+        <v>7080.5789999999997</v>
+      </c>
+      <c r="E13">
+        <v>53317.190999999999</v>
+      </c>
+      <c r="F13">
+        <v>-87.99</v>
+      </c>
+      <c r="G13">
+        <v>0.59399999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C14">
+        <v>29954.053</v>
+      </c>
+      <c r="D14">
+        <v>15210</v>
+      </c>
+      <c r="E14">
+        <v>63551</v>
+      </c>
+      <c r="F14">
+        <v>-89.236000000000004</v>
+      </c>
+      <c r="G14">
+        <v>0.78100000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C15">
+        <v>29001.298999999999</v>
+      </c>
+      <c r="D15">
+        <v>13540</v>
+      </c>
+      <c r="E15">
+        <v>60807.504000000001</v>
+      </c>
+      <c r="F15">
+        <v>-86.399000000000001</v>
+      </c>
+      <c r="G15">
+        <v>0.746</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C16">
+        <v>28735.083999999999</v>
+      </c>
+      <c r="D16">
+        <v>10994</v>
+      </c>
+      <c r="E16">
+        <v>58812.98</v>
+      </c>
+      <c r="F16">
+        <v>-87.838999999999999</v>
+      </c>
+      <c r="G16">
+        <v>0.55200000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C17">
+        <v>20863.269</v>
+      </c>
+      <c r="D17">
+        <v>11057.949000000001</v>
+      </c>
+      <c r="E17">
+        <v>34860.108999999997</v>
+      </c>
+      <c r="F17">
+        <v>-100.739</v>
+      </c>
+      <c r="G17">
+        <v>0.61499999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C18">
+        <v>34234.862000000001</v>
+      </c>
+      <c r="D18">
+        <v>22255.067999999999</v>
+      </c>
+      <c r="E18">
+        <v>49932.75</v>
+      </c>
+      <c r="F18">
+        <v>-90.430999999999997</v>
+      </c>
+      <c r="G18">
+        <v>0.69299999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C19">
+        <v>33819.156000000003</v>
+      </c>
+      <c r="D19">
+        <v>19964.096000000001</v>
+      </c>
+      <c r="E19">
+        <v>57805.046999999999</v>
+      </c>
+      <c r="F19">
+        <v>-90.909000000000006</v>
+      </c>
+      <c r="G19">
+        <v>0.65600000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C20">
+        <v>33386.324000000001</v>
+      </c>
+      <c r="D20">
+        <v>24077.166000000001</v>
+      </c>
+      <c r="E20">
+        <v>56830.16</v>
+      </c>
+      <c r="F20">
+        <v>-87.117000000000004</v>
+      </c>
+      <c r="G20">
+        <v>0.72499999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C21">
+        <v>32697.047999999999</v>
+      </c>
+      <c r="D21">
+        <v>21766.157999999999</v>
+      </c>
+      <c r="E21">
+        <v>53195</v>
+      </c>
+      <c r="F21">
+        <v>-87.325000000000003</v>
+      </c>
+      <c r="G21">
+        <v>0.55800000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C22">
+        <v>32233.819</v>
+      </c>
+      <c r="D22">
+        <v>21442.719000000001</v>
+      </c>
+      <c r="E22">
+        <v>47917.858999999997</v>
+      </c>
+      <c r="F22">
+        <v>-88.995000000000005</v>
+      </c>
+      <c r="G22">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C23">
+        <v>44392.502</v>
+      </c>
+      <c r="D23">
+        <v>27336</v>
+      </c>
+      <c r="E23">
+        <v>57375.457000000002</v>
+      </c>
+      <c r="F23">
+        <v>-88.909000000000006</v>
+      </c>
+      <c r="G23">
+        <v>0.54700000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C24">
+        <v>41767.203000000001</v>
+      </c>
+      <c r="D24">
+        <v>27978</v>
+      </c>
+      <c r="E24">
+        <v>58576.805</v>
+      </c>
+      <c r="F24">
+        <v>-88.838999999999999</v>
+      </c>
+      <c r="G24">
+        <v>0.77100000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C25">
+        <v>42620.008000000002</v>
+      </c>
+      <c r="D25">
+        <v>29972.967000000001</v>
+      </c>
+      <c r="E25">
+        <v>63408.453000000001</v>
+      </c>
+      <c r="F25">
+        <v>-89.075999999999993</v>
+      </c>
+      <c r="G25">
+        <v>0.64600000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C26">
+        <v>41052.864000000001</v>
+      </c>
+      <c r="D26">
+        <v>19175</v>
+      </c>
+      <c r="E26">
+        <v>58351</v>
+      </c>
+      <c r="F26">
+        <v>-88.21</v>
+      </c>
+      <c r="G26">
+        <v>0.66700000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C27">
+        <v>49609.048000000003</v>
+      </c>
+      <c r="D27">
+        <v>30644</v>
+      </c>
+      <c r="E27">
+        <v>64998.074000000001</v>
+      </c>
+      <c r="F27">
+        <v>-89.575999999999993</v>
+      </c>
+      <c r="G27">
+        <v>0.70299999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C28">
+        <v>39785.093999999997</v>
+      </c>
+      <c r="D28">
+        <v>29837.105</v>
+      </c>
+      <c r="E28">
+        <v>51962.421999999999</v>
+      </c>
+      <c r="F28">
+        <v>-88.933000000000007</v>
+      </c>
+      <c r="G28">
+        <v>0.83899999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C29">
+        <v>34260.262999999999</v>
+      </c>
+      <c r="D29">
+        <v>23988.92</v>
+      </c>
+      <c r="E29">
+        <v>45223.440999999999</v>
+      </c>
+      <c r="F29">
+        <v>-89.236000000000004</v>
+      </c>
+      <c r="G29">
+        <v>0.78100000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C30">
+        <v>47797.012000000002</v>
+      </c>
+      <c r="D30">
+        <v>26499</v>
+      </c>
+      <c r="E30">
+        <v>61908.203000000001</v>
+      </c>
+      <c r="F30">
+        <v>-90.486000000000004</v>
+      </c>
+      <c r="G30">
+        <v>0.61499999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C31">
+        <v>48722.209000000003</v>
+      </c>
+      <c r="D31">
+        <v>38804</v>
+      </c>
+      <c r="E31">
+        <v>64415.266000000003</v>
+      </c>
+      <c r="F31">
+        <v>-92.174999999999997</v>
+      </c>
+      <c r="G31">
+        <v>0.82399999999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C32">
+        <v>45770.021000000001</v>
+      </c>
+      <c r="D32">
+        <v>26436</v>
+      </c>
+      <c r="E32">
+        <v>65496</v>
+      </c>
+      <c r="F32">
+        <v>-90</v>
+      </c>
+      <c r="G32">
+        <v>1.458</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C33">
+        <v>48328.309000000001</v>
+      </c>
+      <c r="D33">
+        <v>17087</v>
+      </c>
+      <c r="E33">
+        <v>64964.949000000001</v>
+      </c>
+      <c r="F33">
+        <v>-87.99</v>
+      </c>
+      <c r="G33">
+        <v>1.1879999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C34">
+        <v>47279.273000000001</v>
+      </c>
+      <c r="D34">
+        <v>29879.449000000001</v>
+      </c>
+      <c r="E34">
+        <v>64960.394999999997</v>
+      </c>
+      <c r="F34">
+        <v>-92.305999999999997</v>
+      </c>
+      <c r="G34">
+        <v>1.5529999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C35">
+        <v>46774.250999999997</v>
+      </c>
+      <c r="D35">
+        <v>19849</v>
+      </c>
+      <c r="E35">
+        <v>59322.690999999999</v>
+      </c>
+      <c r="F35">
+        <v>-88.531000000000006</v>
+      </c>
+      <c r="G35">
+        <v>1.6259999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C36">
+        <v>43698.493000000002</v>
+      </c>
+      <c r="D36">
+        <v>29694.085999999999</v>
+      </c>
+      <c r="E36">
+        <v>58614.887000000002</v>
+      </c>
+      <c r="F36">
+        <v>-94.057000000000002</v>
+      </c>
+      <c r="G36">
+        <v>1.472</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="C37">
+        <v>45198.445</v>
+      </c>
+      <c r="D37">
+        <v>37760.508000000002</v>
+      </c>
+      <c r="E37">
+        <v>57295.699000000001</v>
+      </c>
+      <c r="F37">
+        <v>-92.07</v>
+      </c>
+      <c r="G37">
+        <v>0.86499999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C38">
+        <v>49067.618999999999</v>
+      </c>
+      <c r="D38">
+        <v>24015.616999999998</v>
+      </c>
+      <c r="E38">
+        <v>65511.25</v>
+      </c>
+      <c r="F38">
+        <v>-90.385000000000005</v>
+      </c>
+      <c r="G38">
+        <v>1.552</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C39">
+        <v>49952.171999999999</v>
+      </c>
+      <c r="D39">
+        <v>32151.291000000001</v>
+      </c>
+      <c r="E39">
+        <v>65273.237999999998</v>
+      </c>
+      <c r="F39">
+        <v>-89.63</v>
+      </c>
+      <c r="G39">
+        <v>1.615</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="C40">
+        <v>51131.514000000003</v>
+      </c>
+      <c r="D40">
+        <v>37238.714999999997</v>
+      </c>
+      <c r="E40">
+        <v>65528</v>
+      </c>
+      <c r="F40">
+        <v>-90.349000000000004</v>
+      </c>
+      <c r="G40">
+        <v>1.708</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>0.01</v>
+      </c>
+      <c r="C41">
+        <v>46784.434000000001</v>
+      </c>
+      <c r="D41">
+        <v>22516</v>
+      </c>
+      <c r="E41">
+        <v>64067.875</v>
+      </c>
+      <c r="F41">
+        <v>-90.650999999999996</v>
+      </c>
+      <c r="G41">
+        <v>0.91700000000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>0.01</v>
+      </c>
+      <c r="C42">
+        <v>47571.055999999997</v>
+      </c>
+      <c r="D42">
+        <v>32327.449000000001</v>
+      </c>
+      <c r="E42">
+        <v>65355.07</v>
+      </c>
+      <c r="F42">
+        <v>-86.710999999999999</v>
+      </c>
+      <c r="G42">
+        <v>0.90800000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C43">
+        <v>33110.777000000002</v>
+      </c>
+      <c r="D43">
+        <v>22575.467000000001</v>
+      </c>
+      <c r="E43">
+        <v>60543.91</v>
+      </c>
+      <c r="F43">
+        <v>-88.512</v>
+      </c>
+      <c r="G43">
+        <v>1.605</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C44">
+        <v>28870.333999999999</v>
+      </c>
+      <c r="D44">
+        <v>20910</v>
+      </c>
+      <c r="E44">
+        <v>39059.237999999998</v>
+      </c>
+      <c r="F44">
+        <v>-89.236000000000004</v>
+      </c>
+      <c r="G44">
+        <v>1.5629999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C45">
+        <v>31855.239000000001</v>
+      </c>
+      <c r="D45">
+        <v>23203.495999999999</v>
+      </c>
+      <c r="E45">
+        <v>50797.355000000003</v>
+      </c>
+      <c r="F45">
+        <v>-89.731999999999999</v>
+      </c>
+      <c r="G45">
+        <v>2.2290000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C46">
+        <v>31907.503000000001</v>
+      </c>
+      <c r="D46">
+        <v>18372</v>
+      </c>
+      <c r="E46">
+        <v>56923</v>
+      </c>
+      <c r="F46">
+        <v>-88.152000000000001</v>
+      </c>
+      <c r="G46">
+        <v>1.615</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C47">
+        <v>24396.561000000002</v>
+      </c>
+      <c r="D47">
+        <v>13008</v>
+      </c>
+      <c r="E47">
+        <v>31993</v>
+      </c>
+      <c r="F47">
+        <v>-90.83</v>
+      </c>
+      <c r="G47">
+        <v>1.4379999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C48">
+        <v>28692.324000000001</v>
+      </c>
+      <c r="D48">
+        <v>15248.579</v>
+      </c>
+      <c r="E48">
+        <v>41339.156000000003</v>
+      </c>
+      <c r="F48">
+        <v>-88.995000000000005</v>
+      </c>
+      <c r="G48">
+        <v>1.1879999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C49">
+        <v>29175.686000000002</v>
+      </c>
+      <c r="D49">
+        <v>17611.285</v>
+      </c>
+      <c r="E49">
+        <v>45102</v>
+      </c>
+      <c r="F49">
+        <v>-88.861999999999995</v>
+      </c>
+      <c r="G49">
+        <v>1.573</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>1.9E-2</v>
+      </c>
+      <c r="C50">
+        <v>28600.535</v>
+      </c>
+      <c r="D50">
+        <v>20152.895</v>
+      </c>
+      <c r="E50">
+        <v>42607.440999999999</v>
+      </c>
+      <c r="F50">
+        <v>-89.662999999999997</v>
+      </c>
+      <c r="G50">
+        <v>1.7709999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>1.9E-2</v>
+      </c>
+      <c r="C51">
+        <v>29630.880000000001</v>
+      </c>
+      <c r="D51">
+        <v>17050.083999999999</v>
+      </c>
+      <c r="E51">
+        <v>46620.218999999997</v>
+      </c>
+      <c r="F51">
+        <v>-89.676000000000002</v>
+      </c>
+      <c r="G51">
+        <v>1.8440000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C52">
+        <v>25590.922999999999</v>
+      </c>
+      <c r="D52">
+        <v>12750</v>
+      </c>
+      <c r="E52">
+        <v>34918.851999999999</v>
+      </c>
+      <c r="F52">
+        <v>-89.578999999999994</v>
+      </c>
+      <c r="G52">
+        <v>1.417</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="C53">
+        <v>27905.364000000001</v>
+      </c>
+      <c r="D53">
+        <v>15415.332</v>
+      </c>
+      <c r="E53">
+        <v>47200.527000000002</v>
+      </c>
+      <c r="F53">
+        <v>-88.539000000000001</v>
+      </c>
+      <c r="G53">
+        <v>2.0419999999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C54">
+        <v>21660.121999999999</v>
+      </c>
+      <c r="D54">
+        <v>14224.616</v>
+      </c>
+      <c r="E54">
+        <v>35651.25</v>
+      </c>
+      <c r="F54">
+        <v>91.534000000000006</v>
+      </c>
+      <c r="G54">
+        <v>1.167</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="C55">
+        <v>23511.195</v>
+      </c>
+      <c r="D55">
+        <v>14372.103999999999</v>
+      </c>
+      <c r="E55">
+        <v>34845.379000000001</v>
+      </c>
+      <c r="F55">
+        <v>-88.025000000000006</v>
+      </c>
+      <c r="G55">
+        <v>1.2090000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C56">
+        <v>26364.024000000001</v>
+      </c>
+      <c r="D56">
+        <v>16089.141</v>
+      </c>
+      <c r="E56">
+        <v>37301.773000000001</v>
+      </c>
+      <c r="F56">
+        <v>-87.99</v>
+      </c>
+      <c r="G56">
+        <v>1.1879999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C57">
+        <v>25220.587</v>
+      </c>
+      <c r="D57">
+        <v>14870.268</v>
+      </c>
+      <c r="E57">
+        <v>33256.285000000003</v>
+      </c>
+      <c r="F57">
+        <v>-89.488</v>
+      </c>
+      <c r="G57">
+        <v>2.3330000000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C58">
+        <v>31804.527999999998</v>
+      </c>
+      <c r="D58">
+        <v>5911</v>
+      </c>
+      <c r="E58">
+        <v>62965</v>
+      </c>
+      <c r="F58">
+        <v>-90</v>
+      </c>
+      <c r="G58">
+        <v>2.1459999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>0.01</v>
+      </c>
+      <c r="C59">
+        <v>30608.679</v>
+      </c>
+      <c r="D59">
+        <v>8107.5810000000001</v>
+      </c>
+      <c r="E59">
+        <v>61716.608999999997</v>
+      </c>
+      <c r="F59">
+        <v>-89.183999999999997</v>
+      </c>
+      <c r="G59">
+        <v>1.8280000000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>0.01</v>
+      </c>
+      <c r="C60">
+        <v>33167.614999999998</v>
+      </c>
+      <c r="D60">
+        <v>11874.567999999999</v>
+      </c>
+      <c r="E60">
+        <v>63455.637000000002</v>
+      </c>
+      <c r="F60">
+        <v>-88.861000000000004</v>
+      </c>
+      <c r="G60">
+        <v>1.8340000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C61">
+        <v>25673.887999999999</v>
+      </c>
+      <c r="D61">
+        <v>2570</v>
+      </c>
+      <c r="E61">
+        <v>56058.125</v>
+      </c>
+      <c r="F61">
+        <v>-90.894999999999996</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C62">
+        <v>28534.543000000001</v>
+      </c>
+      <c r="D62">
+        <v>7981.77</v>
+      </c>
+      <c r="E62">
+        <v>56297.77</v>
+      </c>
+      <c r="F62">
+        <v>-91.096999999999994</v>
+      </c>
+      <c r="G62">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>0.01</v>
+      </c>
+      <c r="C63">
+        <v>29040.243999999999</v>
+      </c>
+      <c r="D63">
+        <v>5595.9009999999998</v>
+      </c>
+      <c r="E63">
+        <v>60209.086000000003</v>
+      </c>
+      <c r="F63">
+        <v>-88.629000000000005</v>
+      </c>
+      <c r="G63">
+        <v>1.9590000000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>0.01</v>
+      </c>
+      <c r="C64">
+        <v>24991.452000000001</v>
+      </c>
+      <c r="D64">
+        <v>6987.5039999999999</v>
+      </c>
+      <c r="E64">
+        <v>54062.663999999997</v>
+      </c>
+      <c r="F64">
+        <v>-91.290999999999997</v>
+      </c>
+      <c r="G64">
+        <v>1.849</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C65">
+        <v>28542.429</v>
+      </c>
+      <c r="D65">
+        <v>3423.0880000000002</v>
+      </c>
+      <c r="E65">
+        <v>60275.656000000003</v>
+      </c>
+      <c r="F65">
+        <v>-89.296000000000006</v>
+      </c>
+      <c r="G65">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C66">
+        <v>30963.460999999999</v>
+      </c>
+      <c r="D66">
+        <v>8805.7800000000007</v>
+      </c>
+      <c r="E66">
+        <v>60652</v>
+      </c>
+      <c r="F66">
+        <v>-88.426000000000002</v>
+      </c>
+      <c r="G66">
+        <v>0.94799999999999995</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="C67">
+        <v>22681.948</v>
+      </c>
+      <c r="D67">
+        <v>3518.3220000000001</v>
+      </c>
+      <c r="E67">
+        <v>46642.766000000003</v>
+      </c>
+      <c r="F67">
+        <v>91.045000000000002</v>
+      </c>
+      <c r="G67">
+        <v>1.714</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="C68">
+        <v>22684.388999999999</v>
+      </c>
+      <c r="D68">
+        <v>14709.625</v>
+      </c>
+      <c r="E68">
+        <v>33344.800999999999</v>
+      </c>
+      <c r="F68">
+        <v>-90.715999999999994</v>
+      </c>
+      <c r="G68">
+        <v>0.83299999999999996</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="C69">
+        <v>21514.298999999999</v>
+      </c>
+      <c r="D69">
+        <v>14404.050999999999</v>
+      </c>
+      <c r="E69">
+        <v>38612.550999999999</v>
+      </c>
+      <c r="F69">
+        <v>-90.486000000000004</v>
+      </c>
+      <c r="G69">
+        <v>1.2290000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>0.01</v>
+      </c>
+      <c r="C70">
+        <v>30856.105</v>
+      </c>
+      <c r="D70">
+        <v>18972.458999999999</v>
+      </c>
+      <c r="E70">
+        <v>47077.309000000001</v>
+      </c>
+      <c r="F70">
+        <v>-88.683000000000007</v>
+      </c>
+      <c r="G70">
+        <v>0.90600000000000003</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C71">
+        <v>27856.248</v>
+      </c>
+      <c r="D71">
+        <v>15674</v>
+      </c>
+      <c r="E71">
+        <v>53292</v>
+      </c>
+      <c r="F71">
+        <v>-90</v>
+      </c>
+      <c r="G71">
+        <v>1.083</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>0.01</v>
+      </c>
+      <c r="C72">
+        <v>26031.210999999999</v>
+      </c>
+      <c r="D72">
+        <v>15733.742</v>
+      </c>
+      <c r="E72">
+        <v>40322.902000000002</v>
+      </c>
+      <c r="F72">
+        <v>-88.152000000000001</v>
+      </c>
+      <c r="G72">
+        <v>0.96899999999999997</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C73">
+        <v>24537.175999999999</v>
+      </c>
+      <c r="D73">
+        <v>15955.027</v>
+      </c>
+      <c r="E73">
+        <v>34266.741999999998</v>
+      </c>
+      <c r="F73">
+        <v>-89.474000000000004</v>
+      </c>
+      <c r="G73">
+        <v>1.135</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>0.01</v>
+      </c>
+      <c r="C74">
+        <v>29048.52</v>
+      </c>
+      <c r="D74">
+        <v>14250.437</v>
+      </c>
+      <c r="E74">
+        <v>44637.648000000001</v>
+      </c>
+      <c r="F74">
+        <v>-88.171999999999997</v>
+      </c>
+      <c r="G74">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>1.4E-2</v>
+      </c>
+      <c r="C75">
+        <v>27967.941999999999</v>
+      </c>
+      <c r="D75">
+        <v>16829.072</v>
+      </c>
+      <c r="E75">
+        <v>42097.741999999998</v>
+      </c>
+      <c r="F75">
+        <v>-90.457999999999998</v>
+      </c>
+      <c r="G75">
+        <v>1.302</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C76">
+        <v>21193.62</v>
+      </c>
+      <c r="D76">
+        <v>16134.52</v>
+      </c>
+      <c r="E76">
+        <v>29332.800999999999</v>
+      </c>
+      <c r="F76">
+        <v>-92.290999999999997</v>
+      </c>
+      <c r="G76">
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>0.01</v>
+      </c>
+      <c r="C77">
+        <v>25937.967000000001</v>
+      </c>
+      <c r="D77">
+        <v>16798</v>
+      </c>
+      <c r="E77">
+        <v>38965</v>
+      </c>
+      <c r="F77">
+        <v>-90</v>
+      </c>
+      <c r="G77">
+        <v>0.93799999999999994</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G59"/>
   <sheetViews>
@@ -2896,7 +4683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA98C21-BFA7-48B2-9F10-52C8756CF87E}">
   <dimension ref="A1:G66"/>
   <sheetViews>
@@ -3883,7 +5670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DA084A-491B-48A5-B5D9-BC0F1B1B01D2}">
   <dimension ref="A1:G66"/>
   <sheetViews>
@@ -5352,6 +7139,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F342DDA-104A-4EEF-8A3C-7C409C90EFCB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{525792CB-97F9-4114-95A2-B1259B3F0DBF}">
   <dimension ref="A1:G91"/>
   <sheetViews>
@@ -7460,7 +9259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EEB46E7-ADBA-4DB0-9172-CA03D8886C98}">
   <dimension ref="A1:G65"/>
   <sheetViews>
@@ -8320,7 +10119,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{797591B3-680C-4A95-B00F-835CE50BAFB5}">
   <dimension ref="A1:G65"/>
   <sheetViews>
@@ -9811,7 +11610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627C0FF3-AA26-448C-83DB-C05DCB7F71C7}">
   <dimension ref="A1:G66"/>
   <sheetViews>
@@ -11159,7 +12958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5805F89-8E37-459C-8289-55214B36518A}">
   <dimension ref="A1:G65"/>
   <sheetViews>
@@ -12299,7 +14098,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC9B860-4519-42C1-BB62-C3EFC821ECA4}">
   <dimension ref="A1:G66"/>
   <sheetViews>
@@ -13493,7 +15292,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38401ECC-9997-4482-8684-9E720C0D07E9}">
   <dimension ref="A1:G76"/>
   <sheetViews>
@@ -15254,1790 +17053,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C4EBE4-8D22-4729-ACC1-DF5E7929C6E8}">
-  <dimension ref="A1:G77"/>
-  <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G77"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C2">
-        <v>26818.952000000001</v>
-      </c>
-      <c r="D2">
-        <v>16136</v>
-      </c>
-      <c r="E2">
-        <v>45741</v>
-      </c>
-      <c r="F2">
-        <v>-90</v>
-      </c>
-      <c r="G2">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C3">
-        <v>31030.241999999998</v>
-      </c>
-      <c r="D3">
-        <v>13256.61</v>
-      </c>
-      <c r="E3">
-        <v>65504</v>
-      </c>
-      <c r="F3">
-        <v>-91.456000000000003</v>
-      </c>
-      <c r="G3">
-        <v>0.61499999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C4">
-        <v>38263.019</v>
-      </c>
-      <c r="D4">
-        <v>20619.553</v>
-      </c>
-      <c r="E4">
-        <v>65530</v>
-      </c>
-      <c r="F4">
-        <v>-90.754000000000005</v>
-      </c>
-      <c r="G4">
-        <v>0.79200000000000004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C5">
-        <v>26915.843000000001</v>
-      </c>
-      <c r="D5">
-        <v>9787</v>
-      </c>
-      <c r="E5">
-        <v>65068</v>
-      </c>
-      <c r="F5">
-        <v>-89.575999999999993</v>
-      </c>
-      <c r="G5">
-        <v>0.70299999999999996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C6">
-        <v>35671.421000000002</v>
-      </c>
-      <c r="D6">
-        <v>17189</v>
-      </c>
-      <c r="E6">
-        <v>65012.940999999999</v>
-      </c>
-      <c r="F6">
-        <v>-89.144999999999996</v>
-      </c>
-      <c r="G6">
-        <v>0.69799999999999995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C7">
-        <v>30179.966</v>
-      </c>
-      <c r="D7">
-        <v>17040.403999999999</v>
-      </c>
-      <c r="E7">
-        <v>56415.858999999997</v>
-      </c>
-      <c r="F7">
-        <v>-79.478999999999999</v>
-      </c>
-      <c r="G7">
-        <v>0.74199999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C8">
-        <v>18614.136999999999</v>
-      </c>
-      <c r="D8">
-        <v>11648.511</v>
-      </c>
-      <c r="E8">
-        <v>27521</v>
-      </c>
-      <c r="F8">
-        <v>-91.218999999999994</v>
-      </c>
-      <c r="G8">
-        <v>0.49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C9">
-        <v>18364.919999999998</v>
-      </c>
-      <c r="D9">
-        <v>12653.067999999999</v>
-      </c>
-      <c r="E9">
-        <v>28810.9</v>
-      </c>
-      <c r="F9">
-        <v>-89.125</v>
-      </c>
-      <c r="G9">
-        <v>0.68200000000000005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C10">
-        <v>25063.035</v>
-      </c>
-      <c r="D10">
-        <v>12794</v>
-      </c>
-      <c r="E10">
-        <v>50928.983999999997</v>
-      </c>
-      <c r="F10">
-        <v>-88.543999999999997</v>
-      </c>
-      <c r="G10">
-        <v>0.61499999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C11">
-        <v>29180.918000000001</v>
-      </c>
-      <c r="D11">
-        <v>13566.919</v>
-      </c>
-      <c r="E11">
-        <v>55846.195</v>
-      </c>
-      <c r="F11">
-        <v>-88.137</v>
-      </c>
-      <c r="G11">
-        <v>0.64100000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C12">
-        <v>26569.732</v>
-      </c>
-      <c r="D12">
-        <v>5985</v>
-      </c>
-      <c r="E12">
-        <v>49784.866999999998</v>
-      </c>
-      <c r="F12">
-        <v>-90.444000000000003</v>
-      </c>
-      <c r="G12">
-        <v>0.67200000000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C13">
-        <v>26378.094000000001</v>
-      </c>
-      <c r="D13">
-        <v>7080.5789999999997</v>
-      </c>
-      <c r="E13">
-        <v>53317.190999999999</v>
-      </c>
-      <c r="F13">
-        <v>-87.99</v>
-      </c>
-      <c r="G13">
-        <v>0.59399999999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C14">
-        <v>29954.053</v>
-      </c>
-      <c r="D14">
-        <v>15210</v>
-      </c>
-      <c r="E14">
-        <v>63551</v>
-      </c>
-      <c r="F14">
-        <v>-89.236000000000004</v>
-      </c>
-      <c r="G14">
-        <v>0.78100000000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C15">
-        <v>29001.298999999999</v>
-      </c>
-      <c r="D15">
-        <v>13540</v>
-      </c>
-      <c r="E15">
-        <v>60807.504000000001</v>
-      </c>
-      <c r="F15">
-        <v>-86.399000000000001</v>
-      </c>
-      <c r="G15">
-        <v>0.746</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C16">
-        <v>28735.083999999999</v>
-      </c>
-      <c r="D16">
-        <v>10994</v>
-      </c>
-      <c r="E16">
-        <v>58812.98</v>
-      </c>
-      <c r="F16">
-        <v>-87.838999999999999</v>
-      </c>
-      <c r="G16">
-        <v>0.55200000000000005</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C17">
-        <v>20863.269</v>
-      </c>
-      <c r="D17">
-        <v>11057.949000000001</v>
-      </c>
-      <c r="E17">
-        <v>34860.108999999997</v>
-      </c>
-      <c r="F17">
-        <v>-100.739</v>
-      </c>
-      <c r="G17">
-        <v>0.61499999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C18">
-        <v>34234.862000000001</v>
-      </c>
-      <c r="D18">
-        <v>22255.067999999999</v>
-      </c>
-      <c r="E18">
-        <v>49932.75</v>
-      </c>
-      <c r="F18">
-        <v>-90.430999999999997</v>
-      </c>
-      <c r="G18">
-        <v>0.69299999999999995</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C19">
-        <v>33819.156000000003</v>
-      </c>
-      <c r="D19">
-        <v>19964.096000000001</v>
-      </c>
-      <c r="E19">
-        <v>57805.046999999999</v>
-      </c>
-      <c r="F19">
-        <v>-90.909000000000006</v>
-      </c>
-      <c r="G19">
-        <v>0.65600000000000003</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C20">
-        <v>33386.324000000001</v>
-      </c>
-      <c r="D20">
-        <v>24077.166000000001</v>
-      </c>
-      <c r="E20">
-        <v>56830.16</v>
-      </c>
-      <c r="F20">
-        <v>-87.117000000000004</v>
-      </c>
-      <c r="G20">
-        <v>0.72499999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C21">
-        <v>32697.047999999999</v>
-      </c>
-      <c r="D21">
-        <v>21766.157999999999</v>
-      </c>
-      <c r="E21">
-        <v>53195</v>
-      </c>
-      <c r="F21">
-        <v>-87.325000000000003</v>
-      </c>
-      <c r="G21">
-        <v>0.55800000000000005</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C22">
-        <v>32233.819</v>
-      </c>
-      <c r="D22">
-        <v>21442.719000000001</v>
-      </c>
-      <c r="E22">
-        <v>47917.858999999997</v>
-      </c>
-      <c r="F22">
-        <v>-88.995000000000005</v>
-      </c>
-      <c r="G22">
-        <v>0.89100000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C23">
-        <v>44392.502</v>
-      </c>
-      <c r="D23">
-        <v>27336</v>
-      </c>
-      <c r="E23">
-        <v>57375.457000000002</v>
-      </c>
-      <c r="F23">
-        <v>-88.909000000000006</v>
-      </c>
-      <c r="G23">
-        <v>0.54700000000000004</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C24">
-        <v>41767.203000000001</v>
-      </c>
-      <c r="D24">
-        <v>27978</v>
-      </c>
-      <c r="E24">
-        <v>58576.805</v>
-      </c>
-      <c r="F24">
-        <v>-88.838999999999999</v>
-      </c>
-      <c r="G24">
-        <v>0.77100000000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C25">
-        <v>42620.008000000002</v>
-      </c>
-      <c r="D25">
-        <v>29972.967000000001</v>
-      </c>
-      <c r="E25">
-        <v>63408.453000000001</v>
-      </c>
-      <c r="F25">
-        <v>-89.075999999999993</v>
-      </c>
-      <c r="G25">
-        <v>0.64600000000000002</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C26">
-        <v>41052.864000000001</v>
-      </c>
-      <c r="D26">
-        <v>19175</v>
-      </c>
-      <c r="E26">
-        <v>58351</v>
-      </c>
-      <c r="F26">
-        <v>-88.21</v>
-      </c>
-      <c r="G26">
-        <v>0.66700000000000004</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C27">
-        <v>49609.048000000003</v>
-      </c>
-      <c r="D27">
-        <v>30644</v>
-      </c>
-      <c r="E27">
-        <v>64998.074000000001</v>
-      </c>
-      <c r="F27">
-        <v>-89.575999999999993</v>
-      </c>
-      <c r="G27">
-        <v>0.70299999999999996</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C28">
-        <v>39785.093999999997</v>
-      </c>
-      <c r="D28">
-        <v>29837.105</v>
-      </c>
-      <c r="E28">
-        <v>51962.421999999999</v>
-      </c>
-      <c r="F28">
-        <v>-88.933000000000007</v>
-      </c>
-      <c r="G28">
-        <v>0.83899999999999997</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C29">
-        <v>34260.262999999999</v>
-      </c>
-      <c r="D29">
-        <v>23988.92</v>
-      </c>
-      <c r="E29">
-        <v>45223.440999999999</v>
-      </c>
-      <c r="F29">
-        <v>-89.236000000000004</v>
-      </c>
-      <c r="G29">
-        <v>0.78100000000000003</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C30">
-        <v>47797.012000000002</v>
-      </c>
-      <c r="D30">
-        <v>26499</v>
-      </c>
-      <c r="E30">
-        <v>61908.203000000001</v>
-      </c>
-      <c r="F30">
-        <v>-90.486000000000004</v>
-      </c>
-      <c r="G30">
-        <v>0.61499999999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C31">
-        <v>48722.209000000003</v>
-      </c>
-      <c r="D31">
-        <v>38804</v>
-      </c>
-      <c r="E31">
-        <v>64415.266000000003</v>
-      </c>
-      <c r="F31">
-        <v>-92.174999999999997</v>
-      </c>
-      <c r="G31">
-        <v>0.82399999999999995</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="C32">
-        <v>45770.021000000001</v>
-      </c>
-      <c r="D32">
-        <v>26436</v>
-      </c>
-      <c r="E32">
-        <v>65496</v>
-      </c>
-      <c r="F32">
-        <v>-90</v>
-      </c>
-      <c r="G32">
-        <v>1.458</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>1.2E-2</v>
-      </c>
-      <c r="C33">
-        <v>48328.309000000001</v>
-      </c>
-      <c r="D33">
-        <v>17087</v>
-      </c>
-      <c r="E33">
-        <v>64964.949000000001</v>
-      </c>
-      <c r="F33">
-        <v>-87.99</v>
-      </c>
-      <c r="G33">
-        <v>1.1879999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>1.6E-2</v>
-      </c>
-      <c r="C34">
-        <v>47279.273000000001</v>
-      </c>
-      <c r="D34">
-        <v>29879.449000000001</v>
-      </c>
-      <c r="E34">
-        <v>64960.394999999997</v>
-      </c>
-      <c r="F34">
-        <v>-92.305999999999997</v>
-      </c>
-      <c r="G34">
-        <v>1.5529999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="C35">
-        <v>46774.250999999997</v>
-      </c>
-      <c r="D35">
-        <v>19849</v>
-      </c>
-      <c r="E35">
-        <v>59322.690999999999</v>
-      </c>
-      <c r="F35">
-        <v>-88.531000000000006</v>
-      </c>
-      <c r="G35">
-        <v>1.6259999999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="C36">
-        <v>43698.493000000002</v>
-      </c>
-      <c r="D36">
-        <v>29694.085999999999</v>
-      </c>
-      <c r="E36">
-        <v>58614.887000000002</v>
-      </c>
-      <c r="F36">
-        <v>-94.057000000000002</v>
-      </c>
-      <c r="G36">
-        <v>1.472</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="C37">
-        <v>45198.445</v>
-      </c>
-      <c r="D37">
-        <v>37760.508000000002</v>
-      </c>
-      <c r="E37">
-        <v>57295.699000000001</v>
-      </c>
-      <c r="F37">
-        <v>-92.07</v>
-      </c>
-      <c r="G37">
-        <v>0.86499999999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <v>1.6E-2</v>
-      </c>
-      <c r="C38">
-        <v>49067.618999999999</v>
-      </c>
-      <c r="D38">
-        <v>24015.616999999998</v>
-      </c>
-      <c r="E38">
-        <v>65511.25</v>
-      </c>
-      <c r="F38">
-        <v>-90.385000000000005</v>
-      </c>
-      <c r="G38">
-        <v>1.552</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="C39">
-        <v>49952.171999999999</v>
-      </c>
-      <c r="D39">
-        <v>32151.291000000001</v>
-      </c>
-      <c r="E39">
-        <v>65273.237999999998</v>
-      </c>
-      <c r="F39">
-        <v>-89.63</v>
-      </c>
-      <c r="G39">
-        <v>1.615</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="C40">
-        <v>51131.514000000003</v>
-      </c>
-      <c r="D40">
-        <v>37238.714999999997</v>
-      </c>
-      <c r="E40">
-        <v>65528</v>
-      </c>
-      <c r="F40">
-        <v>-90.349000000000004</v>
-      </c>
-      <c r="G40">
-        <v>1.708</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41">
-        <v>0.01</v>
-      </c>
-      <c r="C41">
-        <v>46784.434000000001</v>
-      </c>
-      <c r="D41">
-        <v>22516</v>
-      </c>
-      <c r="E41">
-        <v>64067.875</v>
-      </c>
-      <c r="F41">
-        <v>-90.650999999999996</v>
-      </c>
-      <c r="G41">
-        <v>0.91700000000000004</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42">
-        <v>0.01</v>
-      </c>
-      <c r="C42">
-        <v>47571.055999999997</v>
-      </c>
-      <c r="D42">
-        <v>32327.449000000001</v>
-      </c>
-      <c r="E42">
-        <v>65355.07</v>
-      </c>
-      <c r="F42">
-        <v>-86.710999999999999</v>
-      </c>
-      <c r="G42">
-        <v>0.90800000000000003</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="C43">
-        <v>33110.777000000002</v>
-      </c>
-      <c r="D43">
-        <v>22575.467000000001</v>
-      </c>
-      <c r="E43">
-        <v>60543.91</v>
-      </c>
-      <c r="F43">
-        <v>-88.512</v>
-      </c>
-      <c r="G43">
-        <v>1.605</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44">
-        <v>1.6E-2</v>
-      </c>
-      <c r="C44">
-        <v>28870.333999999999</v>
-      </c>
-      <c r="D44">
-        <v>20910</v>
-      </c>
-      <c r="E44">
-        <v>39059.237999999998</v>
-      </c>
-      <c r="F44">
-        <v>-89.236000000000004</v>
-      </c>
-      <c r="G44">
-        <v>1.5629999999999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45">
-        <v>2.3E-2</v>
-      </c>
-      <c r="C45">
-        <v>31855.239000000001</v>
-      </c>
-      <c r="D45">
-        <v>23203.495999999999</v>
-      </c>
-      <c r="E45">
-        <v>50797.355000000003</v>
-      </c>
-      <c r="F45">
-        <v>-89.731999999999999</v>
-      </c>
-      <c r="G45">
-        <v>2.2290000000000001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="C46">
-        <v>31907.503000000001</v>
-      </c>
-      <c r="D46">
-        <v>18372</v>
-      </c>
-      <c r="E46">
-        <v>56923</v>
-      </c>
-      <c r="F46">
-        <v>-88.152000000000001</v>
-      </c>
-      <c r="G46">
-        <v>1.615</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="C47">
-        <v>24396.561000000002</v>
-      </c>
-      <c r="D47">
-        <v>13008</v>
-      </c>
-      <c r="E47">
-        <v>31993</v>
-      </c>
-      <c r="F47">
-        <v>-90.83</v>
-      </c>
-      <c r="G47">
-        <v>1.4379999999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48">
-        <v>1.2E-2</v>
-      </c>
-      <c r="C48">
-        <v>28692.324000000001</v>
-      </c>
-      <c r="D48">
-        <v>15248.579</v>
-      </c>
-      <c r="E48">
-        <v>41339.156000000003</v>
-      </c>
-      <c r="F48">
-        <v>-88.995000000000005</v>
-      </c>
-      <c r="G48">
-        <v>1.1879999999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49">
-        <v>1.6E-2</v>
-      </c>
-      <c r="C49">
-        <v>29175.686000000002</v>
-      </c>
-      <c r="D49">
-        <v>17611.285</v>
-      </c>
-      <c r="E49">
-        <v>45102</v>
-      </c>
-      <c r="F49">
-        <v>-88.861999999999995</v>
-      </c>
-      <c r="G49">
-        <v>1.573</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="B50">
-        <v>1.9E-2</v>
-      </c>
-      <c r="C50">
-        <v>28600.535</v>
-      </c>
-      <c r="D50">
-        <v>20152.895</v>
-      </c>
-      <c r="E50">
-        <v>42607.440999999999</v>
-      </c>
-      <c r="F50">
-        <v>-89.662999999999997</v>
-      </c>
-      <c r="G50">
-        <v>1.7709999999999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="B51">
-        <v>1.9E-2</v>
-      </c>
-      <c r="C51">
-        <v>29630.880000000001</v>
-      </c>
-      <c r="D51">
-        <v>17050.083999999999</v>
-      </c>
-      <c r="E51">
-        <v>46620.218999999997</v>
-      </c>
-      <c r="F51">
-        <v>-89.676000000000002</v>
-      </c>
-      <c r="G51">
-        <v>1.8440000000000001</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="B52">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="C52">
-        <v>25590.922999999999</v>
-      </c>
-      <c r="D52">
-        <v>12750</v>
-      </c>
-      <c r="E52">
-        <v>34918.851999999999</v>
-      </c>
-      <c r="F52">
-        <v>-89.578999999999994</v>
-      </c>
-      <c r="G52">
-        <v>1.417</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="B53">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="C53">
-        <v>27905.364000000001</v>
-      </c>
-      <c r="D53">
-        <v>15415.332</v>
-      </c>
-      <c r="E53">
-        <v>47200.527000000002</v>
-      </c>
-      <c r="F53">
-        <v>-88.539000000000001</v>
-      </c>
-      <c r="G53">
-        <v>2.0419999999999998</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="B54">
-        <v>1.2E-2</v>
-      </c>
-      <c r="C54">
-        <v>21660.121999999999</v>
-      </c>
-      <c r="D54">
-        <v>14224.616</v>
-      </c>
-      <c r="E54">
-        <v>35651.25</v>
-      </c>
-      <c r="F54">
-        <v>91.534000000000006</v>
-      </c>
-      <c r="G54">
-        <v>1.167</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="B55">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="C55">
-        <v>23511.195</v>
-      </c>
-      <c r="D55">
-        <v>14372.103999999999</v>
-      </c>
-      <c r="E55">
-        <v>34845.379000000001</v>
-      </c>
-      <c r="F55">
-        <v>-88.025000000000006</v>
-      </c>
-      <c r="G55">
-        <v>1.2090000000000001</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56">
-        <v>1.2E-2</v>
-      </c>
-      <c r="C56">
-        <v>26364.024000000001</v>
-      </c>
-      <c r="D56">
-        <v>16089.141</v>
-      </c>
-      <c r="E56">
-        <v>37301.773000000001</v>
-      </c>
-      <c r="F56">
-        <v>-87.99</v>
-      </c>
-      <c r="G56">
-        <v>1.1879999999999999</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="B57">
-        <v>2.4E-2</v>
-      </c>
-      <c r="C57">
-        <v>25220.587</v>
-      </c>
-      <c r="D57">
-        <v>14870.268</v>
-      </c>
-      <c r="E57">
-        <v>33256.285000000003</v>
-      </c>
-      <c r="F57">
-        <v>-89.488</v>
-      </c>
-      <c r="G57">
-        <v>2.3330000000000002</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="B58">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="C58">
-        <v>31804.527999999998</v>
-      </c>
-      <c r="D58">
-        <v>5911</v>
-      </c>
-      <c r="E58">
-        <v>62965</v>
-      </c>
-      <c r="F58">
-        <v>-90</v>
-      </c>
-      <c r="G58">
-        <v>2.1459999999999999</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="B59">
-        <v>0.01</v>
-      </c>
-      <c r="C59">
-        <v>30608.679</v>
-      </c>
-      <c r="D59">
-        <v>8107.5810000000001</v>
-      </c>
-      <c r="E59">
-        <v>61716.608999999997</v>
-      </c>
-      <c r="F59">
-        <v>-89.183999999999997</v>
-      </c>
-      <c r="G59">
-        <v>1.8280000000000001</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="B60">
-        <v>0.01</v>
-      </c>
-      <c r="C60">
-        <v>33167.614999999998</v>
-      </c>
-      <c r="D60">
-        <v>11874.567999999999</v>
-      </c>
-      <c r="E60">
-        <v>63455.637000000002</v>
-      </c>
-      <c r="F60">
-        <v>-88.861000000000004</v>
-      </c>
-      <c r="G60">
-        <v>1.8340000000000001</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C61">
-        <v>25673.887999999999</v>
-      </c>
-      <c r="D61">
-        <v>2570</v>
-      </c>
-      <c r="E61">
-        <v>56058.125</v>
-      </c>
-      <c r="F61">
-        <v>-90.894999999999996</v>
-      </c>
-      <c r="G61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="B62">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="C62">
-        <v>28534.543000000001</v>
-      </c>
-      <c r="D62">
-        <v>7981.77</v>
-      </c>
-      <c r="E62">
-        <v>56297.77</v>
-      </c>
-      <c r="F62">
-        <v>-91.096999999999994</v>
-      </c>
-      <c r="G62">
-        <v>1.36</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="B63">
-        <v>0.01</v>
-      </c>
-      <c r="C63">
-        <v>29040.243999999999</v>
-      </c>
-      <c r="D63">
-        <v>5595.9009999999998</v>
-      </c>
-      <c r="E63">
-        <v>60209.086000000003</v>
-      </c>
-      <c r="F63">
-        <v>-88.629000000000005</v>
-      </c>
-      <c r="G63">
-        <v>1.9590000000000001</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>63</v>
-      </c>
-      <c r="B64">
-        <v>0.01</v>
-      </c>
-      <c r="C64">
-        <v>24991.452000000001</v>
-      </c>
-      <c r="D64">
-        <v>6987.5039999999999</v>
-      </c>
-      <c r="E64">
-        <v>54062.663999999997</v>
-      </c>
-      <c r="F64">
-        <v>-91.290999999999997</v>
-      </c>
-      <c r="G64">
-        <v>1.849</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>64</v>
-      </c>
-      <c r="B65">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="C65">
-        <v>28542.429</v>
-      </c>
-      <c r="D65">
-        <v>3423.0880000000002</v>
-      </c>
-      <c r="E65">
-        <v>60275.656000000003</v>
-      </c>
-      <c r="F65">
-        <v>-89.296000000000006</v>
-      </c>
-      <c r="G65">
-        <v>2.12</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>65</v>
-      </c>
-      <c r="B66">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C66">
-        <v>30963.460999999999</v>
-      </c>
-      <c r="D66">
-        <v>8805.7800000000007</v>
-      </c>
-      <c r="E66">
-        <v>60652</v>
-      </c>
-      <c r="F66">
-        <v>-88.426000000000002</v>
-      </c>
-      <c r="G66">
-        <v>0.94799999999999995</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>66</v>
-      </c>
-      <c r="B67">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="C67">
-        <v>22681.948</v>
-      </c>
-      <c r="D67">
-        <v>3518.3220000000001</v>
-      </c>
-      <c r="E67">
-        <v>46642.766000000003</v>
-      </c>
-      <c r="F67">
-        <v>91.045000000000002</v>
-      </c>
-      <c r="G67">
-        <v>1.714</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>67</v>
-      </c>
-      <c r="B68">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="C68">
-        <v>22684.388999999999</v>
-      </c>
-      <c r="D68">
-        <v>14709.625</v>
-      </c>
-      <c r="E68">
-        <v>33344.800999999999</v>
-      </c>
-      <c r="F68">
-        <v>-90.715999999999994</v>
-      </c>
-      <c r="G68">
-        <v>0.83299999999999996</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>68</v>
-      </c>
-      <c r="B69">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="C69">
-        <v>21514.298999999999</v>
-      </c>
-      <c r="D69">
-        <v>14404.050999999999</v>
-      </c>
-      <c r="E69">
-        <v>38612.550999999999</v>
-      </c>
-      <c r="F69">
-        <v>-90.486000000000004</v>
-      </c>
-      <c r="G69">
-        <v>1.2290000000000001</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>69</v>
-      </c>
-      <c r="B70">
-        <v>0.01</v>
-      </c>
-      <c r="C70">
-        <v>30856.105</v>
-      </c>
-      <c r="D70">
-        <v>18972.458999999999</v>
-      </c>
-      <c r="E70">
-        <v>47077.309000000001</v>
-      </c>
-      <c r="F70">
-        <v>-88.683000000000007</v>
-      </c>
-      <c r="G70">
-        <v>0.90600000000000003</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>70</v>
-      </c>
-      <c r="B71">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="C71">
-        <v>27856.248</v>
-      </c>
-      <c r="D71">
-        <v>15674</v>
-      </c>
-      <c r="E71">
-        <v>53292</v>
-      </c>
-      <c r="F71">
-        <v>-90</v>
-      </c>
-      <c r="G71">
-        <v>1.083</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>71</v>
-      </c>
-      <c r="B72">
-        <v>0.01</v>
-      </c>
-      <c r="C72">
-        <v>26031.210999999999</v>
-      </c>
-      <c r="D72">
-        <v>15733.742</v>
-      </c>
-      <c r="E72">
-        <v>40322.902000000002</v>
-      </c>
-      <c r="F72">
-        <v>-88.152000000000001</v>
-      </c>
-      <c r="G72">
-        <v>0.96899999999999997</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>72</v>
-      </c>
-      <c r="B73">
-        <v>1.2E-2</v>
-      </c>
-      <c r="C73">
-        <v>24537.175999999999</v>
-      </c>
-      <c r="D73">
-        <v>15955.027</v>
-      </c>
-      <c r="E73">
-        <v>34266.741999999998</v>
-      </c>
-      <c r="F73">
-        <v>-89.474000000000004</v>
-      </c>
-      <c r="G73">
-        <v>1.135</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>73</v>
-      </c>
-      <c r="B74">
-        <v>0.01</v>
-      </c>
-      <c r="C74">
-        <v>29048.52</v>
-      </c>
-      <c r="D74">
-        <v>14250.437</v>
-      </c>
-      <c r="E74">
-        <v>44637.648000000001</v>
-      </c>
-      <c r="F74">
-        <v>-88.171999999999997</v>
-      </c>
-      <c r="G74">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>74</v>
-      </c>
-      <c r="B75">
-        <v>1.4E-2</v>
-      </c>
-      <c r="C75">
-        <v>27967.941999999999</v>
-      </c>
-      <c r="D75">
-        <v>16829.072</v>
-      </c>
-      <c r="E75">
-        <v>42097.741999999998</v>
-      </c>
-      <c r="F75">
-        <v>-90.457999999999998</v>
-      </c>
-      <c r="G75">
-        <v>1.302</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>75</v>
-      </c>
-      <c r="B76">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="C76">
-        <v>21193.62</v>
-      </c>
-      <c r="D76">
-        <v>16134.52</v>
-      </c>
-      <c r="E76">
-        <v>29332.800999999999</v>
-      </c>
-      <c r="F76">
-        <v>-92.290999999999997</v>
-      </c>
-      <c r="G76">
-        <v>0.78200000000000003</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>76</v>
-      </c>
-      <c r="B77">
-        <v>0.01</v>
-      </c>
-      <c r="C77">
-        <v>25937.967000000001</v>
-      </c>
-      <c r="D77">
-        <v>16798</v>
-      </c>
-      <c r="E77">
-        <v>38965</v>
-      </c>
-      <c r="F77">
-        <v>-90</v>
-      </c>
-      <c r="G77">
-        <v>0.93799999999999994</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>